<commit_message>
update for BHSF, WISRD, and Intermatic
</commit_message>
<xml_diff>
--- a/DavesSupportSuite.suite/Resources/NonStaffProvider_022425.xlsx
+++ b/DavesSupportSuite.suite/Resources/NonStaffProvider_022425.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="libxl" lastEdited="7" lowestEdited="7" rupBuild="4.5.1"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="564" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="574" uniqueCount="270">
   <si>
     <t>Status</t>
   </si>

</xml_diff>